<commit_message>
updated data file and methods
</commit_message>
<xml_diff>
--- a/version_comparison.xlsx
+++ b/version_comparison.xlsx
@@ -30380,31 +30380,31 @@
       <c r="S545" s="3"/>
     </row>
     <row r="546">
-      <c r="A546" s="6" t="n">
+      <c r="A546" s="4" t="n">
         <v>1142</v>
       </c>
-      <c r="B546" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C546" s="6" t="s">
+      <c r="B546" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C546" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="D546" s="6" t="n">
-        <v>41.325</v>
-      </c>
-      <c r="E546" s="6" t="n">
+      <c r="D546" s="4" t="n">
+        <v>41.325</v>
+      </c>
+      <c r="E546" s="4" t="n">
         <v>-70.566</v>
       </c>
-      <c r="F546" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="G546" s="6" t="s">
+      <c r="F546" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G546" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="H546" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I546" s="6" t="n">
+      <c r="H546" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I546" s="4" t="n">
         <v>0</v>
       </c>
       <c r="J546" s="6"/>
@@ -30431,106 +30431,106 @@
       <c r="S546" s="6"/>
     </row>
     <row r="547">
-      <c r="A547" s="6" t="n">
-        <v>1142</v>
-      </c>
-      <c r="B547" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C547" s="6" t="s">
+      <c r="A547" s="1" t="n">
+        <v>1143</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C547" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="D547" s="6" t="n">
-        <v>41.325</v>
-      </c>
-      <c r="E547" s="6" t="n">
+      <c r="D547" s="1" t="n">
+        <v>41.325</v>
+      </c>
+      <c r="E547" s="1" t="n">
         <v>-70.566</v>
       </c>
-      <c r="F547" s="6" t="n">
+      <c r="F547" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="G547" s="6" t="s">
+      <c r="G547" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="H547" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I547" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J547" s="6"/>
-      <c r="K547" s="4" t="n">
+      <c r="H547" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I547" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J547" s="3"/>
+      <c r="K547" s="1" t="n">
         <v>1.333</v>
       </c>
-      <c r="L547" s="4" t="n">
+      <c r="L547" s="1" t="n">
         <v>1.338</v>
       </c>
-      <c r="M547" s="6"/>
-      <c r="N547" s="4" t="n">
+      <c r="M547" s="3"/>
+      <c r="N547" s="1" t="n">
         <v>0.478</v>
       </c>
-      <c r="O547" s="4" t="n">
+      <c r="O547" s="1" t="n">
         <v>0.466</v>
       </c>
-      <c r="P547" s="6"/>
-      <c r="Q547" s="4" t="n">
+      <c r="P547" s="3"/>
+      <c r="Q547" s="1" t="n">
         <v>0.355</v>
       </c>
-      <c r="R547" s="4" t="n">
+      <c r="R547" s="1" t="n">
         <v>0.431</v>
       </c>
-      <c r="S547" s="6"/>
+      <c r="S547" s="3"/>
     </row>
     <row r="548">
-      <c r="A548" s="1" t="n">
-        <v>1143</v>
-      </c>
-      <c r="B548" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C548" s="1" t="s">
+      <c r="A548" s="4" t="n">
+        <v>1144</v>
+      </c>
+      <c r="B548" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C548" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D548" s="1" t="n">
-        <v>41.325</v>
-      </c>
-      <c r="E548" s="1" t="n">
+      <c r="D548" s="4" t="n">
+        <v>41.325</v>
+      </c>
+      <c r="E548" s="4" t="n">
         <v>-70.566</v>
       </c>
-      <c r="F548" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G548" s="1" t="s">
+      <c r="F548" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G548" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="H548" s="1" t="n">
+      <c r="H548" s="4" t="n">
         <v>0.092</v>
       </c>
-      <c r="I548" s="1" t="n">
+      <c r="I548" s="4" t="n">
         <v>0.041</v>
       </c>
-      <c r="J548" s="3"/>
-      <c r="K548" s="1" t="n">
+      <c r="J548" s="6"/>
+      <c r="K548" s="4" t="n">
         <v>1.753</v>
       </c>
-      <c r="L548" s="1" t="n">
+      <c r="L548" s="4" t="n">
         <v>1.791</v>
       </c>
-      <c r="M548" s="3"/>
-      <c r="N548" s="1" t="n">
+      <c r="M548" s="6"/>
+      <c r="N548" s="4" t="n">
         <v>0.564</v>
       </c>
-      <c r="O548" s="1" t="n">
+      <c r="O548" s="4" t="n">
         <v>0.568</v>
       </c>
-      <c r="P548" s="3"/>
-      <c r="Q548" s="1" t="n">
+      <c r="P548" s="6"/>
+      <c r="Q548" s="4" t="n">
         <v>1.433</v>
       </c>
-      <c r="R548" s="1" t="n">
+      <c r="R548" s="4" t="n">
         <v>1.398</v>
       </c>
-      <c r="S548" s="3"/>
+      <c r="S548" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>